<commit_message>
conducted kruskal wallis test
</commit_message>
<xml_diff>
--- a/Vorstudie-Data/SurveyCircle/Results-SurveyCircle.xlsx
+++ b/Vorstudie-Data/SurveyCircle/Results-SurveyCircle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasoberfrank/Documents/Uni Hamburg/Master-Thesis/Statistics-Virtual-Agents-MA/SurveyCircle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasoberfrank/Documents/Uni Hamburg/Master-Thesis/Statistics-Virtual-Agents-MA/Vorstudie-Data/SurveyCircle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13166EC9-E6EC-844D-A4F4-6C25EB0FA3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C22BB-8DE9-C94B-A570-3BC1145413EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="19440" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49440" yWindow="500" windowWidth="19200" windowHeight="23500" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bewertung virtueller Charaktere" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="225">
   <si>
     <t>id. Antwort ID</t>
   </si>
@@ -584,6 +584,117 @@
   </si>
   <si>
     <t>ER06ER21</t>
+  </si>
+  <si>
+    <t>2024-06-30 15:00:59</t>
+  </si>
+  <si>
+    <t>2024-06-30 15:02:39</t>
+  </si>
+  <si>
+    <t>AA11AA11</t>
+  </si>
+  <si>
+    <t>2024-07-01 11:15:29</t>
+  </si>
+  <si>
+    <t>2024-07-01 11:08:48</t>
+  </si>
+  <si>
+    <t>ER05AS22</t>
+  </si>
+  <si>
+    <t>2024-07-01 23:32:59</t>
+  </si>
+  <si>
+    <t>2024-07-01 23:23:13</t>
+  </si>
+  <si>
+    <t>H34VY</t>
+  </si>
+  <si>
+    <t>Nicht binär</t>
+  </si>
+  <si>
+    <t>Realschulabschluss</t>
+  </si>
+  <si>
+    <t>2024-07-02 13:25:58</t>
+  </si>
+  <si>
+    <t>2024-07-02 12:01:11</t>
+  </si>
+  <si>
+    <t>KA06SZ19</t>
+  </si>
+  <si>
+    <t>Mehrmals in der Woche</t>
+  </si>
+  <si>
+    <t>Master-Abschluss</t>
+  </si>
+  <si>
+    <t>2024-07-02 14:09:28</t>
+  </si>
+  <si>
+    <t>2024-07-02 14:01:43</t>
+  </si>
+  <si>
+    <t>NN06US28</t>
+  </si>
+  <si>
+    <t>2024-07-02 22:30:41</t>
+  </si>
+  <si>
+    <t>2024-07-02 22:25:21</t>
+  </si>
+  <si>
+    <t>NG6NZ26</t>
+  </si>
+  <si>
+    <t>Täglich</t>
+  </si>
+  <si>
+    <t>2024-07-03 21:51:39</t>
+  </si>
+  <si>
+    <t>2024-07-03 21:39:50</t>
+  </si>
+  <si>
+    <t>PA08LF19</t>
+  </si>
+  <si>
+    <t>2024-07-05 14:12:49</t>
+  </si>
+  <si>
+    <t>2024-07-05 14:05:09</t>
+  </si>
+  <si>
+    <t>LL06US20</t>
+  </si>
+  <si>
+    <t>2024-07-05 14:16:00</t>
+  </si>
+  <si>
+    <t>2024-07-05 14:07:07</t>
+  </si>
+  <si>
+    <t>CK09AS17</t>
+  </si>
+  <si>
+    <t>2024-07-06 20:05:57</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2024-07-07 15:54:30</t>
+  </si>
+  <si>
+    <t>2024-07-07 15:49:13</t>
+  </si>
+  <si>
+    <t>FD05DF09</t>
   </si>
 </sst>
 </file>
@@ -961,18 +1072,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FA8"/>
+  <dimension ref="A1:FA19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C27" sqref="C26:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1024" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:157" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:157" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1556,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>89</v>
       </c>
@@ -1876,7 +1987,7 @@
         <v>13.74</v>
       </c>
     </row>
-    <row r="3" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>90</v>
       </c>
@@ -2304,7 +2415,7 @@
         <v>38.85</v>
       </c>
     </row>
-    <row r="4" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>92</v>
       </c>
@@ -2732,7 +2843,7 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="5" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>93</v>
       </c>
@@ -3163,7 +3274,7 @@
         <v>13.31</v>
       </c>
     </row>
-    <row r="6" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>94</v>
       </c>
@@ -3594,7 +3705,7 @@
         <v>13.33</v>
       </c>
     </row>
-    <row r="7" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>95</v>
       </c>
@@ -4025,7 +4136,7 @@
         <v>19.96</v>
       </c>
     </row>
-    <row r="8" spans="1:157" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>96</v>
       </c>
@@ -4454,6 +4565,4006 @@
       </c>
       <c r="EW8" s="1">
         <v>32.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:157" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>97</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9">
+        <v>1822045478</v>
+      </c>
+      <c r="F9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" t="s">
+        <v>190</v>
+      </c>
+      <c r="J9" t="s">
+        <v>162</v>
+      </c>
+      <c r="BS9">
+        <v>1</v>
+      </c>
+      <c r="BT9">
+        <v>1</v>
+      </c>
+      <c r="BU9">
+        <v>1</v>
+      </c>
+      <c r="BV9">
+        <v>1</v>
+      </c>
+      <c r="BW9">
+        <v>1</v>
+      </c>
+      <c r="BX9">
+        <v>1</v>
+      </c>
+      <c r="BY9">
+        <v>1</v>
+      </c>
+      <c r="BZ9">
+        <v>1</v>
+      </c>
+      <c r="CA9">
+        <v>3</v>
+      </c>
+      <c r="CB9">
+        <v>3</v>
+      </c>
+      <c r="CC9">
+        <v>3</v>
+      </c>
+      <c r="CD9">
+        <v>3</v>
+      </c>
+      <c r="CE9">
+        <v>3</v>
+      </c>
+      <c r="CF9">
+        <v>3</v>
+      </c>
+      <c r="CG9">
+        <v>3</v>
+      </c>
+      <c r="CH9">
+        <v>3</v>
+      </c>
+      <c r="CI9">
+        <v>3</v>
+      </c>
+      <c r="CJ9">
+        <v>3</v>
+      </c>
+      <c r="CK9">
+        <v>3</v>
+      </c>
+      <c r="CL9">
+        <v>3</v>
+      </c>
+      <c r="EG9">
+        <v>100.88</v>
+      </c>
+      <c r="EH9">
+        <v>49.29</v>
+      </c>
+      <c r="EQ9">
+        <v>51.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="1">
+        <v>110888121</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K10" s="1">
+        <v>3</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2</v>
+      </c>
+      <c r="R10" s="1">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1">
+        <v>3</v>
+      </c>
+      <c r="U10" s="1">
+        <v>2</v>
+      </c>
+      <c r="V10" s="1">
+        <v>3</v>
+      </c>
+      <c r="W10" s="1">
+        <v>3</v>
+      </c>
+      <c r="X10" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AX10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AZ10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC10" s="1">
+        <v>4</v>
+      </c>
+      <c r="BD10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI10" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BU10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BV10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BW10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BX10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CE10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CI10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CM10" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CO10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP10" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CR10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CS10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CT10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CU10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DB10" s="1">
+        <v>2</v>
+      </c>
+      <c r="DC10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DD10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF10" s="1">
+        <v>4</v>
+      </c>
+      <c r="DG10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DH10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DM10" s="1">
+        <v>2</v>
+      </c>
+      <c r="DN10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO10" s="1">
+        <v>2</v>
+      </c>
+      <c r="DP10" s="1">
+        <v>4</v>
+      </c>
+      <c r="DQ10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DR10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DT10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DV10" s="1">
+        <v>4</v>
+      </c>
+      <c r="DW10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DY10" s="1">
+        <v>3</v>
+      </c>
+      <c r="DZ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="EA10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EB10" s="1">
+        <v>28</v>
+      </c>
+      <c r="EC10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EE10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG10" s="1">
+        <v>405.72</v>
+      </c>
+      <c r="EH10" s="1">
+        <v>123.87</v>
+      </c>
+      <c r="EK10" s="1">
+        <v>47.83</v>
+      </c>
+      <c r="EM10" s="1">
+        <v>36.82</v>
+      </c>
+      <c r="EO10" s="1">
+        <v>48.43</v>
+      </c>
+      <c r="EQ10" s="1">
+        <v>38.61</v>
+      </c>
+      <c r="ES10" s="1">
+        <v>60.24</v>
+      </c>
+      <c r="EU10" s="1">
+        <v>35.83</v>
+      </c>
+      <c r="EW10" s="1">
+        <v>14.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>99</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1133233627</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>3</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>5</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>3</v>
+      </c>
+      <c r="V11" s="1">
+        <v>3</v>
+      </c>
+      <c r="W11" s="1">
+        <v>3</v>
+      </c>
+      <c r="X11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AU11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW11" s="1">
+        <v>5</v>
+      </c>
+      <c r="AX11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA11" s="1">
+        <v>5</v>
+      </c>
+      <c r="BB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC11" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD11" s="1">
+        <v>5</v>
+      </c>
+      <c r="BE11" s="1">
+        <v>5</v>
+      </c>
+      <c r="BF11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG11" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH11" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO11" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BS11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BU11" s="1">
+        <v>4</v>
+      </c>
+      <c r="BV11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BX11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CG11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CJ11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CL11" s="1">
+        <v>5</v>
+      </c>
+      <c r="CM11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CO11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CP11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CR11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CS11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CU11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CV11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CZ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DB11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DC11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DD11" s="1">
+        <v>2</v>
+      </c>
+      <c r="DE11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF11" s="1">
+        <v>2</v>
+      </c>
+      <c r="DG11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL11" s="1">
+        <v>2</v>
+      </c>
+      <c r="DM11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO11" s="1">
+        <v>5</v>
+      </c>
+      <c r="DP11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DQ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DR11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DT11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DU11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DV11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DW11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX11" s="1">
+        <v>2</v>
+      </c>
+      <c r="DY11" s="1">
+        <v>2</v>
+      </c>
+      <c r="DZ11" s="1">
+        <v>5</v>
+      </c>
+      <c r="EA11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="EB11" s="1">
+        <v>34</v>
+      </c>
+      <c r="EC11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="EE11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="EG11" s="1">
+        <v>589.83000000000004</v>
+      </c>
+      <c r="EH11" s="1">
+        <v>83.91</v>
+      </c>
+      <c r="EK11" s="1">
+        <v>85.82</v>
+      </c>
+      <c r="EM11" s="1">
+        <v>133.22999999999999</v>
+      </c>
+      <c r="EO11" s="1">
+        <v>54.73</v>
+      </c>
+      <c r="EQ11" s="1">
+        <v>72</v>
+      </c>
+      <c r="ES11" s="1">
+        <v>71.37</v>
+      </c>
+      <c r="EU11" s="1">
+        <v>59.63</v>
+      </c>
+      <c r="EW11" s="1">
+        <v>29.14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="1">
+        <v>261038668</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2</v>
+      </c>
+      <c r="P12" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>2</v>
+      </c>
+      <c r="T12" s="1">
+        <v>2</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2</v>
+      </c>
+      <c r="V12" s="1">
+        <v>2</v>
+      </c>
+      <c r="W12" s="1">
+        <v>3</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AO12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AY12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AZ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BD12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ12" s="1">
+        <v>5</v>
+      </c>
+      <c r="BK12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BL12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM12" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BU12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BV12" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW12" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE12" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH12" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CJ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CL12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CM12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CU12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CX12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CY12" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DB12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DC12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DE12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DH12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DL12" s="1">
+        <v>2</v>
+      </c>
+      <c r="DM12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DN12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO12" s="1">
+        <v>4</v>
+      </c>
+      <c r="DP12" s="1">
+        <v>4</v>
+      </c>
+      <c r="DQ12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DR12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS12" s="1">
+        <v>4</v>
+      </c>
+      <c r="DT12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DV12" s="1">
+        <v>4</v>
+      </c>
+      <c r="DW12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX12" s="1">
+        <v>3</v>
+      </c>
+      <c r="DY12" s="1">
+        <v>4</v>
+      </c>
+      <c r="DZ12" s="1">
+        <v>2</v>
+      </c>
+      <c r="EA12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="EB12" s="1">
+        <v>25</v>
+      </c>
+      <c r="EC12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EE12" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="EG12" s="1">
+        <v>5089.74</v>
+      </c>
+      <c r="EH12" s="1">
+        <v>930.13</v>
+      </c>
+      <c r="EK12" s="1">
+        <v>54</v>
+      </c>
+      <c r="EM12" s="1">
+        <v>43.56</v>
+      </c>
+      <c r="EO12" s="1">
+        <v>43.26</v>
+      </c>
+      <c r="EQ12" s="1">
+        <v>3901.74</v>
+      </c>
+      <c r="ES12" s="1">
+        <v>50.55</v>
+      </c>
+      <c r="EU12" s="1">
+        <v>41.1</v>
+      </c>
+      <c r="EW12" s="1">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>101</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1172568913</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1">
+        <v>4</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3</v>
+      </c>
+      <c r="O13" s="1">
+        <v>3</v>
+      </c>
+      <c r="P13" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>4</v>
+      </c>
+      <c r="R13" s="1">
+        <v>3</v>
+      </c>
+      <c r="S13" s="1">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1">
+        <v>4</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>3</v>
+      </c>
+      <c r="W13" s="1">
+        <v>3</v>
+      </c>
+      <c r="X13" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AU13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AY13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AZ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BC13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG13" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BK13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BL13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BM13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BT13" s="1">
+        <v>4</v>
+      </c>
+      <c r="BU13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BV13" s="1">
+        <v>3</v>
+      </c>
+      <c r="BW13" s="1">
+        <v>4</v>
+      </c>
+      <c r="BX13" s="1">
+        <v>4</v>
+      </c>
+      <c r="BY13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CF13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CG13" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CJ13" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CL13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CM13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CO13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CR13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CS13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CT13" s="1">
+        <v>4</v>
+      </c>
+      <c r="CU13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CY13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CZ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DA13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DB13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DC13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DE13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DF13" s="1">
+        <v>5</v>
+      </c>
+      <c r="DG13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DK13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DM13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DP13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DQ13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DR13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DS13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DT13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DU13" s="1">
+        <v>1</v>
+      </c>
+      <c r="DV13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DW13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX13" s="1">
+        <v>2</v>
+      </c>
+      <c r="DY13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DZ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="EA13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="EB13" s="1">
+        <v>43</v>
+      </c>
+      <c r="EC13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EE13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG13" s="1">
+        <v>468.34</v>
+      </c>
+      <c r="EH13" s="1">
+        <v>150.69</v>
+      </c>
+      <c r="EK13" s="1">
+        <v>45.25</v>
+      </c>
+      <c r="EM13" s="1">
+        <v>47.88</v>
+      </c>
+      <c r="EO13" s="1">
+        <v>44.68</v>
+      </c>
+      <c r="EQ13" s="1">
+        <v>45.09</v>
+      </c>
+      <c r="ES13" s="1">
+        <v>80.930000000000007</v>
+      </c>
+      <c r="EU13" s="1">
+        <v>38.76</v>
+      </c>
+      <c r="EW13" s="1">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>102</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="1">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="1">
+        <v>545970933</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <v>3</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>3</v>
+      </c>
+      <c r="P14" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2</v>
+      </c>
+      <c r="R14" s="1">
+        <v>3</v>
+      </c>
+      <c r="S14" s="1">
+        <v>4</v>
+      </c>
+      <c r="T14" s="1">
+        <v>3</v>
+      </c>
+      <c r="U14" s="1">
+        <v>4</v>
+      </c>
+      <c r="V14" s="1">
+        <v>3</v>
+      </c>
+      <c r="W14" s="1">
+        <v>3</v>
+      </c>
+      <c r="X14" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AT14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AU14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX14" s="1">
+        <v>4</v>
+      </c>
+      <c r="AY14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BB14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI14" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ14" s="1">
+        <v>4</v>
+      </c>
+      <c r="BK14" s="1">
+        <v>4</v>
+      </c>
+      <c r="BL14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM14" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BS14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT14" s="1">
+        <v>4</v>
+      </c>
+      <c r="BU14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BV14" s="1">
+        <v>2</v>
+      </c>
+      <c r="BW14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BX14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ14" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC14" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CE14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CM14" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN14" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO14" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP14" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CR14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CS14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CT14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CU14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CV14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CW14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CX14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY14" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DB14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DC14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DM14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DP14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DQ14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DR14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DS14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DT14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DU14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DV14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DW14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DX14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DY14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DZ14" s="1">
+        <v>2</v>
+      </c>
+      <c r="EA14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="EB14" s="1">
+        <v>21</v>
+      </c>
+      <c r="EC14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EE14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="EG14" s="1">
+        <v>324.88</v>
+      </c>
+      <c r="EH14" s="1">
+        <v>82.79</v>
+      </c>
+      <c r="EK14" s="1">
+        <v>40.72</v>
+      </c>
+      <c r="EM14" s="1">
+        <v>34.729999999999997</v>
+      </c>
+      <c r="EO14" s="1">
+        <v>47.17</v>
+      </c>
+      <c r="EQ14" s="1">
+        <v>32.619999999999997</v>
+      </c>
+      <c r="ES14" s="1">
+        <v>27.91</v>
+      </c>
+      <c r="EU14" s="1">
+        <v>39.590000000000003</v>
+      </c>
+      <c r="EW14" s="1">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>103</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1825403750</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>3</v>
+      </c>
+      <c r="P15" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>3</v>
+      </c>
+      <c r="R15" s="1">
+        <v>3</v>
+      </c>
+      <c r="S15" s="1">
+        <v>3</v>
+      </c>
+      <c r="T15" s="1">
+        <v>3</v>
+      </c>
+      <c r="U15" s="1">
+        <v>3</v>
+      </c>
+      <c r="V15" s="1">
+        <v>3</v>
+      </c>
+      <c r="W15" s="1">
+        <v>3</v>
+      </c>
+      <c r="X15" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="1">
+        <v>5</v>
+      </c>
+      <c r="AK15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AN15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AZ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BB15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BC15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BD15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BF15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BG15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BK15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BL15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BT15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BU15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BV15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BW15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BX15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BY15" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ15" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC15" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CE15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF15" s="1">
+        <v>4</v>
+      </c>
+      <c r="CG15" s="1">
+        <v>4</v>
+      </c>
+      <c r="CH15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CM15" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CR15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CS15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CT15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CU15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CV15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY15" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DB15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DC15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DG15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DL15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DM15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN15" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DP15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DQ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DR15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DT15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DU15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DV15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DW15" s="1">
+        <v>2</v>
+      </c>
+      <c r="DX15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DY15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DZ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="EA15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EB15" s="1">
+        <v>35</v>
+      </c>
+      <c r="EC15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EE15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG15" s="1">
+        <v>712.35</v>
+      </c>
+      <c r="EH15" s="1">
+        <v>172.66</v>
+      </c>
+      <c r="EK15" s="1">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="EM15" s="1">
+        <v>150.94999999999999</v>
+      </c>
+      <c r="EO15" s="1">
+        <v>51.59</v>
+      </c>
+      <c r="EQ15" s="1">
+        <v>76.52</v>
+      </c>
+      <c r="ES15" s="1">
+        <v>70.03</v>
+      </c>
+      <c r="EU15" s="1">
+        <v>77.58</v>
+      </c>
+      <c r="EW15" s="1">
+        <v>36.840000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:157" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>104</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="1">
+        <v>875935629</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>2</v>
+      </c>
+      <c r="R16" s="1">
+        <v>1</v>
+      </c>
+      <c r="S16" s="1">
+        <v>2</v>
+      </c>
+      <c r="T16" s="1">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1">
+        <v>3</v>
+      </c>
+      <c r="V16" s="1">
+        <v>4</v>
+      </c>
+      <c r="W16" s="1">
+        <v>4</v>
+      </c>
+      <c r="X16" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AS16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AU16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AX16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AY16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AZ16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BB16" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BD16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BG16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BK16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BL16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BM16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BN16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BO16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BS16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BU16" s="1">
+        <v>4</v>
+      </c>
+      <c r="BV16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BW16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BX16" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CB16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CC16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CE16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CF16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CG16" s="1">
+        <v>5</v>
+      </c>
+      <c r="CH16" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CJ16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CK16" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CM16" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO16" s="1">
+        <v>3</v>
+      </c>
+      <c r="CP16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CR16" s="1">
+        <v>3</v>
+      </c>
+      <c r="CS16" s="1">
+        <v>3</v>
+      </c>
+      <c r="CT16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CU16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CV16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW16" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CY16" s="1">
+        <v>4</v>
+      </c>
+      <c r="CZ16" s="1">
+        <v>4</v>
+      </c>
+      <c r="DA16" s="1">
+        <v>4</v>
+      </c>
+      <c r="DB16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DC16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DD16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DE16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DJ16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DM16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DN16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DP16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DQ16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DR16" s="1">
+        <v>4</v>
+      </c>
+      <c r="DS16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DT16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DV16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DW16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DY16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DZ16" s="1">
+        <v>3</v>
+      </c>
+      <c r="EA16" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EB16" s="1">
+        <v>29</v>
+      </c>
+      <c r="EC16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EE16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG16" s="1">
+        <v>465.08</v>
+      </c>
+      <c r="EH16" s="1">
+        <v>84.62</v>
+      </c>
+      <c r="EK16" s="1">
+        <v>127.9</v>
+      </c>
+      <c r="EM16" s="1">
+        <v>49.75</v>
+      </c>
+      <c r="EO16" s="1">
+        <v>42.55</v>
+      </c>
+      <c r="EQ16" s="1">
+        <v>40.43</v>
+      </c>
+      <c r="ES16" s="1">
+        <v>48.08</v>
+      </c>
+      <c r="EU16" s="1">
+        <v>58.89</v>
+      </c>
+      <c r="EW16" s="1">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:153" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1543712531</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K17" s="1">
+        <v>2</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4</v>
+      </c>
+      <c r="M17" s="1">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1">
+        <v>2</v>
+      </c>
+      <c r="O17" s="1">
+        <v>4</v>
+      </c>
+      <c r="P17" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>4</v>
+      </c>
+      <c r="R17" s="1">
+        <v>3</v>
+      </c>
+      <c r="S17" s="1">
+        <v>4</v>
+      </c>
+      <c r="T17" s="1">
+        <v>3</v>
+      </c>
+      <c r="U17" s="1">
+        <v>4</v>
+      </c>
+      <c r="V17" s="1">
+        <v>4</v>
+      </c>
+      <c r="W17" s="1">
+        <v>4</v>
+      </c>
+      <c r="X17" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AU17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AY17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AZ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BB17" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BF17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BK17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS17" s="1">
+        <v>3</v>
+      </c>
+      <c r="BT17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BU17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BV17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BW17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BX17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BY17" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CB17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD17" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CJ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CL17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CM17" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CO17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CP17" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CR17" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS17" s="1">
+        <v>4</v>
+      </c>
+      <c r="CT17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CU17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CV17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CW17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CX17" s="1">
+        <v>2</v>
+      </c>
+      <c r="CY17" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DB17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DC17" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF17" s="1">
+        <v>4</v>
+      </c>
+      <c r="DG17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI17" s="1">
+        <v>2</v>
+      </c>
+      <c r="DJ17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DM17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DN17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DP17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DQ17" s="1">
+        <v>2</v>
+      </c>
+      <c r="DR17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS17" s="1">
+        <v>2</v>
+      </c>
+      <c r="DT17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DV17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DW17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DX17" s="1">
+        <v>3</v>
+      </c>
+      <c r="DY17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DZ17" s="1">
+        <v>3</v>
+      </c>
+      <c r="EA17" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EB17" s="1">
+        <v>26</v>
+      </c>
+      <c r="EC17" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EE17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="EG17" s="1">
+        <v>536.36</v>
+      </c>
+      <c r="EH17" s="1">
+        <v>129.91999999999999</v>
+      </c>
+      <c r="EK17" s="1">
+        <v>61.51</v>
+      </c>
+      <c r="EM17" s="1">
+        <v>46.42</v>
+      </c>
+      <c r="EO17" s="1">
+        <v>70.16</v>
+      </c>
+      <c r="EQ17" s="1">
+        <v>69.16</v>
+      </c>
+      <c r="ES17" s="1">
+        <v>78.22</v>
+      </c>
+      <c r="EU17" s="1">
+        <v>62.47</v>
+      </c>
+      <c r="EW17" s="1">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:153" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18">
+        <v>931694907</v>
+      </c>
+      <c r="F18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G18" t="s">
+        <v>220</v>
+      </c>
+      <c r="H18" t="s">
+        <v>160</v>
+      </c>
+      <c r="J18" t="s">
+        <v>221</v>
+      </c>
+      <c r="EG18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:153" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>107</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1670764455</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2</v>
+      </c>
+      <c r="S19" s="1">
+        <v>3</v>
+      </c>
+      <c r="T19" s="1">
+        <v>2</v>
+      </c>
+      <c r="U19" s="1">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1">
+        <v>3</v>
+      </c>
+      <c r="W19" s="1">
+        <v>3</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY19" s="1">
+        <v>3</v>
+      </c>
+      <c r="AZ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BB19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BK19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BL19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BN19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BR19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BS19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BT19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BU19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BV19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BW19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BX19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CA19" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB19" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CE19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CM19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CN19" s="1">
+        <v>5</v>
+      </c>
+      <c r="CO19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP19" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CT19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CU19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CV19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CW19" s="1">
+        <v>1</v>
+      </c>
+      <c r="CX19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY19" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DB19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DC19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DE19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DF19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DH19" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DJ19" s="1">
+        <v>2</v>
+      </c>
+      <c r="DK19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DL19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DM19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DN19" s="1">
+        <v>2</v>
+      </c>
+      <c r="DO19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DP19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DQ19" s="1">
+        <v>5</v>
+      </c>
+      <c r="DR19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DS19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DT19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DU19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DV19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DW19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DX19" s="1">
+        <v>2</v>
+      </c>
+      <c r="DY19" s="1">
+        <v>4</v>
+      </c>
+      <c r="DZ19" s="1">
+        <v>2</v>
+      </c>
+      <c r="EA19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EB19" s="1">
+        <v>40</v>
+      </c>
+      <c r="EC19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EE19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG19" s="1">
+        <v>321.51</v>
+      </c>
+      <c r="EH19" s="1">
+        <v>26.79</v>
+      </c>
+      <c r="EK19" s="1">
+        <v>42.75</v>
+      </c>
+      <c r="EM19" s="1">
+        <v>50.8</v>
+      </c>
+      <c r="EO19" s="1">
+        <v>52.39</v>
+      </c>
+      <c r="EQ19" s="1">
+        <v>47.69</v>
+      </c>
+      <c r="ES19" s="1">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="EU19" s="1">
+        <v>44.23</v>
+      </c>
+      <c r="EW19" s="1">
+        <v>16.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data and conducted analysis
</commit_message>
<xml_diff>
--- a/Vorstudie-Data/SurveyCircle/Results-SurveyCircle.xlsx
+++ b/Vorstudie-Data/SurveyCircle/Results-SurveyCircle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasoberfrank/Documents/Uni Hamburg/Master-Thesis/Statistics-Virtual-Agents-MA/Vorstudie-Data/SurveyCircle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C22BB-8DE9-C94B-A570-3BC1145413EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96F923D-CCAD-894B-B1CF-179A770C7C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49440" yWindow="500" windowWidth="19200" windowHeight="23500" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="19200" windowHeight="23500" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bewertung virtueller Charaktere" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="231">
   <si>
     <t>id. Antwort ID</t>
   </si>
@@ -695,6 +695,24 @@
   </si>
   <si>
     <t>FD05DF09</t>
+  </si>
+  <si>
+    <t>2024-07-08 14:59:01</t>
+  </si>
+  <si>
+    <t>2024-07-08 14:38:23</t>
+  </si>
+  <si>
+    <t>ER03PH21</t>
+  </si>
+  <si>
+    <t>2024-07-08 18:39:49</t>
+  </si>
+  <si>
+    <t>2024-07-08 18:29:07</t>
+  </si>
+  <si>
+    <t>ER05AS27</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FA19"/>
+  <dimension ref="A1:FA21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C26:C27"/>
+      <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8567,6 +8585,868 @@
         <v>16.38</v>
       </c>
     </row>
+    <row r="20" spans="1:153" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>108</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="1">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="1">
+        <v>240827508</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>2</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
+        <v>2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>4</v>
+      </c>
+      <c r="R20" s="1">
+        <v>2</v>
+      </c>
+      <c r="S20" s="1">
+        <v>2</v>
+      </c>
+      <c r="T20" s="1">
+        <v>2</v>
+      </c>
+      <c r="U20" s="1">
+        <v>2</v>
+      </c>
+      <c r="V20" s="1">
+        <v>3</v>
+      </c>
+      <c r="W20" s="1">
+        <v>3</v>
+      </c>
+      <c r="X20" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AU20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BB20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BK20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BL20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BO20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BT20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BU20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BV20" s="1">
+        <v>2</v>
+      </c>
+      <c r="BW20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BX20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BY20" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA20" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CE20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CF20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CG20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CH20" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI20" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CK20" s="1">
+        <v>1</v>
+      </c>
+      <c r="CL20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CM20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN20" s="1">
+        <v>1</v>
+      </c>
+      <c r="CO20" s="1">
+        <v>3</v>
+      </c>
+      <c r="CP20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CR20" s="1">
+        <v>3</v>
+      </c>
+      <c r="CS20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CT20" s="1">
+        <v>3</v>
+      </c>
+      <c r="CU20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CW20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CY20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CZ20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DB20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DC20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DE20" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DG20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DM20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DP20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DQ20" s="1">
+        <v>4</v>
+      </c>
+      <c r="DR20" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS20" s="1">
+        <v>3</v>
+      </c>
+      <c r="DT20" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU20" s="1">
+        <v>2</v>
+      </c>
+      <c r="DV20" s="1">
+        <v>4</v>
+      </c>
+      <c r="DW20" s="1">
+        <v>4</v>
+      </c>
+      <c r="DX20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DY20" s="1">
+        <v>3</v>
+      </c>
+      <c r="DZ20" s="1">
+        <v>3</v>
+      </c>
+      <c r="EA20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="EB20" s="1">
+        <v>27</v>
+      </c>
+      <c r="EC20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EE20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG20" s="1">
+        <v>1241.02</v>
+      </c>
+      <c r="EH20" s="1">
+        <v>73.47</v>
+      </c>
+      <c r="EK20" s="1">
+        <v>55.21</v>
+      </c>
+      <c r="EM20" s="1">
+        <v>48.87</v>
+      </c>
+      <c r="EO20" s="1">
+        <v>51.21</v>
+      </c>
+      <c r="EQ20" s="1">
+        <v>64.34</v>
+      </c>
+      <c r="ES20" s="1">
+        <v>79.97</v>
+      </c>
+      <c r="EU20" s="1">
+        <v>54.45</v>
+      </c>
+      <c r="EW20" s="1">
+        <v>813.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:153" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>109</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1119587364</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>4</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2</v>
+      </c>
+      <c r="O21" s="1">
+        <v>3</v>
+      </c>
+      <c r="P21" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>4</v>
+      </c>
+      <c r="R21" s="1">
+        <v>3</v>
+      </c>
+      <c r="S21" s="1">
+        <v>2</v>
+      </c>
+      <c r="T21" s="1">
+        <v>2</v>
+      </c>
+      <c r="U21" s="1">
+        <v>4</v>
+      </c>
+      <c r="V21" s="1">
+        <v>4</v>
+      </c>
+      <c r="W21" s="1">
+        <v>5</v>
+      </c>
+      <c r="X21" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AT21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AZ21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BK21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BL21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM21" s="1">
+        <v>4</v>
+      </c>
+      <c r="BN21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BO21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BS21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BT21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BU21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BV21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BX21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CL21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CM21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CS21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CT21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CU21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CV21" s="1">
+        <v>1</v>
+      </c>
+      <c r="CW21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX21" s="1">
+        <v>2</v>
+      </c>
+      <c r="CY21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DB21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DC21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DD21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DE21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DI21" s="1">
+        <v>2</v>
+      </c>
+      <c r="DJ21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DK21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DL21" s="1">
+        <v>2</v>
+      </c>
+      <c r="DM21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DN21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DO21" s="1">
+        <v>2</v>
+      </c>
+      <c r="DP21" s="1">
+        <v>2</v>
+      </c>
+      <c r="DQ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DR21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DS21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DT21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DU21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DV21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DW21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DX21" s="1">
+        <v>3</v>
+      </c>
+      <c r="DY21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DZ21" s="1">
+        <v>4</v>
+      </c>
+      <c r="EA21" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EB21" s="1">
+        <v>26</v>
+      </c>
+      <c r="EC21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EE21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EG21" s="1">
+        <v>646.21</v>
+      </c>
+      <c r="EH21" s="1">
+        <v>104.69</v>
+      </c>
+      <c r="EK21" s="1">
+        <v>73.67</v>
+      </c>
+      <c r="EM21" s="1">
+        <v>61.5</v>
+      </c>
+      <c r="EO21" s="1">
+        <v>65.41</v>
+      </c>
+      <c r="EQ21" s="1">
+        <v>233.25</v>
+      </c>
+      <c r="ES21" s="1">
+        <v>47.44</v>
+      </c>
+      <c r="EU21" s="1">
+        <v>45.61</v>
+      </c>
+      <c r="EW21" s="1">
+        <v>14.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>